<commit_message>
Added test case & cleaned SwsFormClick test
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-sws.xlsx
+++ b/test-data/webanalytics-sws.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4C058CFC-9064-448E-B003-57492DC15413}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5CDEEDE4-3CD7-4D87-A2BE-A2ABBEFA6C9C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SitewideSearch" sheetId="1" r:id="rId1"/>
+    <sheet name="SitewideSearchEn" sheetId="1" r:id="rId1"/>
     <sheet name="SitewideSearchEs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
-  <si>
-    <t>breast</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>ipilimumab</t>
   </si>
@@ -37,9 +34,6 @@
     <t>Kaposi's sarcoma</t>
   </si>
   <si>
-    <t>CancerTerm</t>
-  </si>
-  <si>
     <t>BestBet</t>
   </si>
   <si>
@@ -55,9 +49,6 @@
     <t>glioma</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>[F-18]HX4</t>
   </si>
   <si>
@@ -67,9 +58,6 @@
     <t xml:space="preserve">abdominoperineal resection </t>
   </si>
   <si>
-    <t>Dr. Norman E. Sharpless</t>
-  </si>
-  <si>
     <t>LiveHelp</t>
   </si>
   <si>
@@ -82,9 +70,6 @@
     <t>cáncer</t>
   </si>
   <si>
-    <t>cáncer de hígado</t>
-  </si>
-  <si>
     <t>safingol</t>
   </si>
   <si>
@@ -94,10 +79,25 @@
     <t>macrófago</t>
   </si>
   <si>
-    <t>dermis</t>
-  </si>
-  <si>
     <t>argle-bargle or foofaraw</t>
+  </si>
+  <si>
+    <t>ResultType</t>
+  </si>
+  <si>
+    <t>BestBetAndDefinition</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>stereostatic radiosurgery</t>
+  </si>
+  <si>
+    <t>argle-bargle o foofaraw</t>
+  </si>
+  <si>
+    <t>SearchTerm</t>
   </si>
 </sst>
 </file>
@@ -147,11 +147,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,82 +465,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="228" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>250</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2">
-        <v>250</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3"/>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -551,60 +581,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6634F395-7540-4542-954F-5DFBBE6DB702}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More descriptive AssertTrue() messages
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-sws.xlsx
+++ b/test-data/webanalytics-sws.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5CDEEDE4-3CD7-4D87-A2BE-A2ABBEFA6C9C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12756" windowHeight="2640"/>
   </bookViews>
   <sheets>
     <sheet name="SitewideSearchEn" sheetId="1" r:id="rId1"/>
@@ -55,9 +54,6 @@
     <t>10001110101 10001110101</t>
   </si>
   <si>
-    <t xml:space="preserve">abdominoperineal resection </t>
-  </si>
-  <si>
     <t>LiveHelp</t>
   </si>
   <si>
@@ -98,12 +94,15 @@
   </si>
   <si>
     <t>SearchTerm</t>
+  </si>
+  <si>
+    <t>abdominoperineal resection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -464,68 +463,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>250</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -533,39 +532,39 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -580,71 +579,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6634F395-7540-4542-954F-5DFBBE6DB702}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
       <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -652,23 +651,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>

</xml_diff>